<commit_message>
Fixed close / minimise / hiding. Control buttons added.
</commit_message>
<xml_diff>
--- a/HyperX USB Packets.xlsx
+++ b/HyperX USB Packets.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\GitHub\Cloud3Status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B436F1-D9C7-4AEA-A876-0207BD790872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD146F7-715B-4A7B-8C1C-20F87C6C0312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0B3B112F-29EA-4F4F-9525-A57DEB696B3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Responses" sheetId="3" r:id="rId2"/>
+    <sheet name="Button Requests" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>Unmuted</t>
   </si>
@@ -233,6 +234,30 @@
   </si>
   <si>
     <t>Battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66 03 00 </t>
+  </si>
+  <si>
+    <t>MIC ON</t>
+  </si>
+  <si>
+    <t>66 03 01</t>
+  </si>
+  <si>
+    <t>MIC OFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66 01 01 </t>
+  </si>
+  <si>
+    <t>SIDETONE ON</t>
+  </si>
+  <si>
+    <t>66 01 00</t>
+  </si>
+  <si>
+    <t>SIDETONE OFF</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1038,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,4 +1227,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE1583F-0D3A-4E6D-B0DA-240A037DD621}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>